<commit_message>
Updates to BOM files
</commit_message>
<xml_diff>
--- a/reference/hardware/Pro/MX5 PNP_BOM.xlsx
+++ b/reference/hardware/Pro/MX5 PNP_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="256">
   <si>
     <t>Value</t>
   </si>
@@ -317,12 +317,6 @@
     <t>Mouser Import</t>
   </si>
   <si>
-    <t>CL21F104ZBCNNNC</t>
-  </si>
-  <si>
-    <t>1276-1007-1-ND</t>
-  </si>
-  <si>
     <t>CL21B224KOCNNNC</t>
   </si>
   <si>
@@ -332,18 +326,12 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>Y5V</t>
-  </si>
-  <si>
     <t>CL21 Series 0.22 uF 16 V ±10 % Tolerance X7R SMT Multilayer Ceramic Capacitor</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>CL21 Series 0.1uF 50 V -20/+80% Tolerance Y5V SMT Multilayer Ceramic Capacitor</t>
-  </si>
-  <si>
     <t>C11</t>
   </si>
   <si>
@@ -452,9 +440,6 @@
     <t>VJ0805V224ZXXCW1BC</t>
   </si>
   <si>
-    <t>C0805T104K5RALTU</t>
-  </si>
-  <si>
     <t>MM3Z5V1ST1G</t>
   </si>
   <si>
@@ -617,10 +602,6 @@
     <t>MC33814</t>
   </si>
   <si>
-    <t xml:space="preserve">841-MC33814AE
-</t>
-  </si>
-  <si>
     <t>MC33814AE-ND</t>
   </si>
   <si>
@@ -799,6 +780,21 @@
   </si>
   <si>
     <t>D1,D2,D3,D4</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>311-1140-1-ND</t>
+  </si>
+  <si>
+    <t>603-CC805KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>841-MC33814AE</t>
   </si>
 </sst>
 </file>
@@ -1043,12 +1039,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1061,6 +1051,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1456,13 +1452,13 @@
   </sheetPr>
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="102" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="66.83203125" customWidth="1"/>
@@ -1476,7 +1472,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1486,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1535,7 +1531,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1552,7 +1548,7 @@
       <c r="O2" s="3"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4" t="str">
-        <f>IF(NOT(J2=""),A2&amp;","&amp;J2,"")</f>
+        <f t="shared" ref="Q2:Q48" si="0">IF(NOT(J2=""),A2&amp;","&amp;J2,"")</f>
         <v/>
       </c>
       <c r="R2" t="str">
@@ -1561,98 +1557,98 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="21">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>104</v>
+        <v>251</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>96</v>
+        <v>252</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>97</v>
+        <v>253</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>141</v>
+        <v>254</v>
       </c>
       <c r="L3" s="5">
-        <v>0.14000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="M3" s="5">
         <v>0.1</v>
       </c>
       <c r="N3" s="6">
-        <f>L3*A3</f>
-        <v>0.98000000000000009</v>
+        <f t="shared" ref="N3:N11" si="1">L3*A3</f>
+        <v>0.70000000000000007</v>
       </c>
       <c r="O3" s="6">
-        <f>M3*A3</f>
+        <f t="shared" ref="O3:O11" si="2">M3*A3</f>
         <v>0.70000000000000007</v>
       </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="4" t="str">
-        <f>IF(NOT(J3=""),A3&amp;","&amp;J3,"")</f>
-        <v>7,1276-1007-1-ND</v>
+        <f t="shared" si="0"/>
+        <v>7,311-1140-1-ND</v>
       </c>
       <c r="R3" t="str">
-        <f>"Capacitor - " &amp;A3&amp;"x "&amp;C3</f>
+        <f t="shared" ref="R3:R11" si="3">"Capacitor - " &amp;A3&amp;"x "&amp;C3</f>
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
       <c r="S3" t="str">
-        <f>IF(NOT(K3=""),K3&amp;"|"&amp;A3,"")</f>
-        <v>C0805T104K5RALTU|7</v>
+        <f t="shared" ref="S3:S45" si="4">IF(NOT(K3=""),K3&amp;"|"&amp;A3,"")</f>
+        <v>603-CC805KRX7R9BB104|7</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="21">
         <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="L4" s="5">
         <v>0.12</v>
@@ -1661,40 +1657,40 @@
         <v>0.1</v>
       </c>
       <c r="N4" s="6">
-        <f>L4*A4</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="O4" s="6">
-        <f>M4*A4</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="str">
-        <f>IF(NOT(J4=""),A4&amp;","&amp;J4,"")</f>
+        <f t="shared" si="0"/>
         <v>5,1276-1284-1-ND</v>
       </c>
       <c r="R4" t="str">
-        <f>"Capacitor - " &amp;A4&amp;"x "&amp;C4</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 5x 0.22uF</v>
       </c>
       <c r="S4" t="str">
-        <f>IF(NOT(K4=""),K4&amp;"|"&amp;A4,"")</f>
+        <f t="shared" si="4"/>
         <v>VJ0805V224ZXXCW1BC|5</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="21">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>8</v>
@@ -1707,13 +1703,13 @@
         <v>71</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L5" s="5">
         <v>0.1</v>
@@ -1722,40 +1718,40 @@
         <v>0.1</v>
       </c>
       <c r="N5" s="6">
-        <f>L5*A5</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="O5" s="6">
-        <f>M5*A5</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="str">
-        <f>IF(NOT(J5=""),A5&amp;","&amp;J5,"")</f>
+        <f t="shared" si="0"/>
         <v>1,311-1133-1-ND</v>
       </c>
       <c r="R5" t="str">
-        <f>"Capacitor - " &amp;A5&amp;"x "&amp;C5</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 1x 4.7nF</v>
       </c>
       <c r="S5" t="str">
-        <f>IF(NOT(K5=""),K5&amp;"|"&amp;A5,"")</f>
+        <f t="shared" si="4"/>
         <v>603-CC805KRX7R9BB472|1</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="21">
         <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>8</v>
@@ -1768,13 +1764,13 @@
         <v>71</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L6" s="5">
         <v>0.1</v>
@@ -1783,40 +1779,40 @@
         <v>0.1</v>
       </c>
       <c r="N6" s="6">
-        <f>L6*A6</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="O6" s="6">
-        <f>M6*A6</f>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="str">
-        <f>IF(NOT(J6=""),A6&amp;","&amp;J6,"")</f>
+        <f t="shared" si="0"/>
         <v>2,311-1365-1-ND</v>
       </c>
       <c r="R6" t="str">
-        <f>"Capacitor - " &amp;A6&amp;"x "&amp;C6</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 2x 1uF</v>
       </c>
       <c r="S6" t="str">
-        <f>IF(NOT(K6=""),K6&amp;"|"&amp;A6,"")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 603-CC805KKX7R7BB105|2</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
-        <f t="shared" ref="A7:A9" si="0">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
+      <c r="A7" s="21">
+        <f t="shared" ref="A7:A9" si="5">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>8</v>
@@ -1829,13 +1825,13 @@
         <v>71</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L7" s="5">
         <v>0.1</v>
@@ -1844,59 +1840,59 @@
         <v>0.1</v>
       </c>
       <c r="N7" s="6">
-        <f>L7*A7</f>
+        <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="O7" s="6">
-        <f>M7*A7</f>
+        <f t="shared" si="2"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="str">
-        <f>IF(NOT(J7=""),A7&amp;","&amp;J7,"")</f>
+        <f t="shared" si="0"/>
         <v>3,399-1249-1-ND</v>
       </c>
       <c r="R7" t="str">
-        <f>"Capacitor - " &amp;A7&amp;"x "&amp;C7</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 3x 0.1uF</v>
       </c>
       <c r="S7" t="str">
-        <f>IF(NOT(K7=""),K7&amp;"|"&amp;A7,"")</f>
+        <f t="shared" si="4"/>
         <v>80-C1206104K5RAC7867|3</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
-        <f t="shared" si="0"/>
+      <c r="A8" s="21">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="L8" s="5">
         <v>0.54</v>
@@ -1905,30 +1901,30 @@
         <v>0.47</v>
       </c>
       <c r="N8" s="6">
-        <f>L8*A8</f>
+        <f t="shared" si="1"/>
         <v>1.08</v>
       </c>
       <c r="O8" s="6">
-        <f>M8*A8</f>
+        <f t="shared" si="2"/>
         <v>0.94</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="str">
-        <f>IF(NOT(J8=""),A8&amp;","&amp;J8,"")</f>
+        <f t="shared" si="0"/>
         <v>2,478-1692-1-ND</v>
       </c>
       <c r="R8" t="str">
-        <f>"Capacitor - " &amp;A8&amp;"x "&amp;C8</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 2x 47uF</v>
       </c>
       <c r="S8" t="str">
-        <f>IF(NOT(K8=""),K8&amp;"|"&amp;A8,"")</f>
+        <f t="shared" si="4"/>
         <v>581-TAJB476K006R|2</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
-        <f t="shared" si="0"/>
+      <c r="A9" s="21">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1938,10 +1934,10 @@
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
@@ -1951,13 +1947,13 @@
         <v>71</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L9" s="5">
         <v>2.21</v>
@@ -1966,29 +1962,29 @@
         <v>2.21</v>
       </c>
       <c r="N9" s="6">
-        <f>L9*A9</f>
+        <f t="shared" si="1"/>
         <v>2.21</v>
       </c>
       <c r="O9" s="6">
-        <f>M9*A9</f>
+        <f t="shared" si="2"/>
         <v>2.21</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="str">
-        <f>IF(NOT(J9=""),A9&amp;","&amp;J9,"")</f>
+        <f t="shared" si="0"/>
         <v>1,399-8361-1-ND</v>
       </c>
       <c r="R9" t="str">
-        <f>"Capacitor - " &amp;A9&amp;"x "&amp;C9</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 1x 10uF</v>
       </c>
       <c r="S9" t="str">
-        <f>IF(NOT(K9=""),K9&amp;"|"&amp;A9,"")</f>
+        <f t="shared" si="4"/>
         <v>80-T491D106K050|1</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="21">
         <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
         <v>1</v>
       </c>
@@ -1996,10 +1992,10 @@
         <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>8</v>
@@ -2012,13 +2008,13 @@
         <v>71</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L10" s="5">
         <v>0.1</v>
@@ -2027,40 +2023,40 @@
         <v>0.1</v>
       </c>
       <c r="N10" s="6">
-        <f>L10*A10</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="O10" s="6">
-        <f>M10*A10</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="str">
-        <f>IF(NOT(J10=""),A10&amp;","&amp;J10,"")</f>
+        <f t="shared" si="0"/>
         <v>1,311-1124-1-ND</v>
       </c>
       <c r="R10" t="str">
-        <f>"Capacitor - " &amp;A10&amp;"x "&amp;C10</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 1x 470pF</v>
       </c>
       <c r="S10" t="str">
-        <f>IF(NOT(K10=""),K10&amp;"|"&amp;A10,"")</f>
+        <f t="shared" si="4"/>
         <v>603-CC805KRX7R9BB471|1</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="21">
         <f>LEN(B11)-LEN(SUBSTITUTE(B11,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>8</v>
@@ -2073,13 +2069,13 @@
         <v>71</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="L11" s="5">
         <v>0.1</v>
@@ -2088,29 +2084,29 @@
         <v>0.1</v>
       </c>
       <c r="N11" s="6">
-        <f>L11*A11</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="O11" s="6">
-        <f>M11*A11</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="str">
-        <f>IF(NOT(J11=""),A11&amp;","&amp;J11,"")</f>
+        <f t="shared" si="0"/>
         <v>1,311-1136-1-ND</v>
       </c>
       <c r="R11" t="str">
-        <f>"Capacitor - " &amp;A11&amp;"x "&amp;C11</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 1x 10nF</v>
       </c>
       <c r="S11" t="str">
-        <f>IF(NOT(K11=""),K11&amp;"|"&amp;A11,"")</f>
+        <f t="shared" si="4"/>
         <v>603-CC805KRX7R9BB103|1</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2127,24 +2123,24 @@
       <c r="O12" s="6"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="str">
-        <f>IF(NOT(J12=""),A12&amp;","&amp;J12,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S12" t="str">
-        <f>IF(NOT(K12=""),K12&amp;"|"&amp;A12,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
-        <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
+      <c r="A13" s="21">
+        <f t="shared" ref="A13:A18" si="6">LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>13</v>
@@ -2175,43 +2171,43 @@
         <v>0.43</v>
       </c>
       <c r="N13" s="6">
-        <f>L13*A13</f>
+        <f t="shared" ref="N13:N18" si="7">L13*A13</f>
         <v>0.68</v>
       </c>
       <c r="O13" s="6">
-        <f>M13*A13</f>
+        <f t="shared" ref="O13:O18" si="8">M13*A13</f>
         <v>0.86</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="str">
-        <f>IF(NOT(J13=""),A13&amp;","&amp;J13,"")</f>
+        <f t="shared" si="0"/>
         <v>2,1N5919BGOS-ND</v>
       </c>
       <c r="R13" t="str">
-        <f>"Diode - " &amp;A13&amp;"x "&amp;C13</f>
+        <f t="shared" ref="R13:R18" si="9">"Diode - " &amp;A13&amp;"x "&amp;C13</f>
         <v>Diode - 2x 5.6V Zener</v>
       </c>
       <c r="S13" t="str">
-        <f>IF(NOT(K13=""),K13&amp;"|"&amp;A13,"")</f>
+        <f t="shared" si="4"/>
         <v>863-1N5919BRLG|2</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23">
-        <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
+      <c r="A14" s="21">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
@@ -2221,13 +2217,13 @@
         <v>71</v>
       </c>
       <c r="I14" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="L14" s="5">
         <v>0.14000000000000001</v>
@@ -2236,57 +2232,57 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="N14" s="6">
-        <f>L14*A14</f>
+        <f t="shared" si="7"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="O14" s="6">
-        <f>M14*A14</f>
+        <f t="shared" si="8"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="str">
-        <f>IF(NOT(J14=""),A14&amp;","&amp;J14,"")</f>
+        <f t="shared" si="0"/>
         <v>2,MM3Z5V1ST1GOSCT-ND</v>
       </c>
       <c r="R14" t="str">
-        <f>"Diode - " &amp;A14&amp;"x "&amp;C14</f>
+        <f t="shared" si="9"/>
         <v>Diode - 2x 5.1V Zener</v>
       </c>
       <c r="S14" t="str">
-        <f>IF(NOT(K14=""),K14&amp;"|"&amp;A14,"")</f>
+        <f t="shared" si="4"/>
         <v>863-MM3Z5V1ST1G|2</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
-        <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
+      <c r="A15" s="21">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="L15" s="5">
         <v>0.14000000000000001</v>
@@ -2295,34 +2291,34 @@
         <v>0.13</v>
       </c>
       <c r="N15" s="6">
-        <f>L15*A15</f>
+        <f t="shared" si="7"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="O15" s="6">
-        <f>M15*A15</f>
+        <f t="shared" si="8"/>
         <v>0.52</v>
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="str">
-        <f>IF(NOT(J15=""),A15&amp;","&amp;J15,"")</f>
+        <f t="shared" si="0"/>
         <v>4,1N4448WXTPMSCT-ND</v>
       </c>
       <c r="R15" t="str">
-        <f>"Diode - " &amp;A15&amp;"x "&amp;C15</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">Diode - 4x </v>
       </c>
       <c r="S15" t="str">
-        <f>IF(NOT(K15=""),K15&amp;"|"&amp;A15,"")</f>
+        <f t="shared" si="4"/>
         <v>833-1N4448WX-TP|4</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
-        <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
+      <c r="A16" s="21">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>66</v>
@@ -2356,59 +2352,59 @@
         <v>0.39</v>
       </c>
       <c r="N16" s="6">
-        <f>L16*A16</f>
+        <f t="shared" si="7"/>
         <v>0.39</v>
       </c>
       <c r="O16" s="6">
-        <f>M16*A16</f>
+        <f t="shared" si="8"/>
         <v>0.39</v>
       </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="str">
-        <f>IF(NOT(J16=""),A16&amp;","&amp;J16,"")</f>
+        <f t="shared" si="0"/>
         <v>1,1N5818-TPCT-ND</v>
       </c>
       <c r="R16" t="str">
-        <f>"Diode - " &amp;A16&amp;"x "&amp;C16</f>
+        <f t="shared" si="9"/>
         <v>Diode - 1x 1N5818-TP Schottky</v>
       </c>
       <c r="S16" t="str">
-        <f>IF(NOT(K16=""),K16&amp;"|"&amp;A16,"")</f>
+        <f t="shared" si="4"/>
         <v>833-1N5818-TP|1</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23">
-        <f>LEN(B17)-LEN(SUBSTITUTE(B17,",",""))+1</f>
+      <c r="A17" s="21">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>72</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L17" s="5">
         <v>0.39</v>
@@ -2417,30 +2413,30 @@
         <v>0.41</v>
       </c>
       <c r="N17" s="6">
-        <f>L17*A17</f>
+        <f t="shared" si="7"/>
         <v>0.39</v>
       </c>
       <c r="O17" s="6">
-        <f>M17*A17</f>
+        <f t="shared" si="8"/>
         <v>0.41</v>
       </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="4" t="str">
-        <f>IF(NOT(J17=""),A17&amp;","&amp;J17,"")</f>
+        <f t="shared" si="0"/>
         <v>1,B0540WSDICT-ND</v>
       </c>
       <c r="R17" t="str">
-        <f>"Diode - " &amp;A17&amp;"x "&amp;C17</f>
+        <f t="shared" si="9"/>
         <v>Diode - 1x Schottky</v>
       </c>
       <c r="S17" t="str">
-        <f>IF(NOT(K17=""),K17&amp;"|"&amp;A17,"")</f>
+        <f t="shared" si="4"/>
         <v>621-B0540WS-7|1</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23">
-        <f>LEN(B18)-LEN(SUBSTITUTE(B18,",",""))+1</f>
+      <c r="A18" s="21">
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -2450,26 +2446,26 @@
         <v>22</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E18" s="3">
         <v>805</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>72</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="L18" s="5">
         <v>0.26</v>
@@ -2478,29 +2474,29 @@
         <v>0.24</v>
       </c>
       <c r="N18" s="6">
-        <f>L18*A18</f>
+        <f t="shared" si="7"/>
         <v>2.08</v>
       </c>
       <c r="O18" s="6">
-        <f>M18*A18</f>
+        <f t="shared" si="8"/>
         <v>1.92</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="str">
-        <f>IF(NOT(J18=""),A18&amp;","&amp;J18,"")</f>
+        <f t="shared" si="0"/>
         <v>8,475-1415-1-ND</v>
       </c>
       <c r="R18" t="str">
-        <f>"Diode - " &amp;A18&amp;"x "&amp;C18</f>
+        <f t="shared" si="9"/>
         <v>Diode - 8x LED-Red</v>
       </c>
       <c r="S18" t="str">
-        <f>IF(NOT(K18=""),K18&amp;"|"&amp;A18,"")</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 720-LHR974-LP-1|8</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2517,20 +2513,20 @@
       <c r="O19" s="6"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="str">
-        <f>IF(NOT(J19=""),A19&amp;","&amp;J19,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="R19" t="str">
-        <f>A19&amp;"x "&amp;C19</f>
+        <f t="shared" ref="R19:R29" si="10">A19&amp;"x "&amp;C19</f>
         <v xml:space="preserve">x </v>
       </c>
       <c r="S19" t="str">
-        <f>IF(NOT(K19=""),K19&amp;"|"&amp;A19,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23">
+      <c r="A20" s="21">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2577,20 +2573,20 @@
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="str">
-        <f>IF(NOT(J20=""),A20&amp;","&amp;J20,"")</f>
+        <f t="shared" si="0"/>
         <v>1,P7307-ND</v>
       </c>
       <c r="R20" t="str">
-        <f>A20&amp;"x "&amp;C20</f>
+        <f t="shared" si="10"/>
         <v>1x Surge Protection</v>
       </c>
       <c r="S20" t="str">
-        <f>IF(NOT(K20=""),K20&amp;"|"&amp;A20,"")</f>
+        <f t="shared" si="4"/>
         <v>667-ERZ-V14D220|1</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2607,30 +2603,30 @@
       <c r="O21" s="6"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="str">
-        <f>IF(NOT(J21=""),A21&amp;","&amp;J21,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="R21" t="str">
-        <f>A21&amp;"x "&amp;C21</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">x </v>
       </c>
       <c r="S21" t="str">
-        <f>IF(NOT(K21=""),K21&amp;"|"&amp;A21,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23">
+      <c r="A22" s="21">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -2641,13 +2637,13 @@
         <v>71</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="L22" s="5">
         <v>9.06</v>
@@ -2665,20 +2661,20 @@
       </c>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="str">
-        <f>IF(NOT(J22=""),A22&amp;","&amp;J22,"")</f>
+        <f t="shared" si="0"/>
         <v>1,174917-7-ND</v>
       </c>
       <c r="R22" t="str">
-        <f>A22&amp;"x "&amp;C22</f>
+        <f t="shared" si="10"/>
         <v>1x Denso-48</v>
       </c>
       <c r="S22" t="str">
-        <f>IF(NOT(K22=""),K22&amp;"|"&amp;A22,"")</f>
+        <f t="shared" si="4"/>
         <v>571-174917-7|1</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23">
+      <c r="A23" s="21">
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2721,20 +2717,20 @@
       </c>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="str">
-        <f>IF(NOT(J23=""),A23&amp;","&amp;J23,"")</f>
+        <f t="shared" si="0"/>
         <v>5,3M9580-ND</v>
       </c>
       <c r="R23" t="str">
-        <f>A23&amp;"x "&amp;C23</f>
+        <f t="shared" si="10"/>
         <v>5x Jumper</v>
       </c>
       <c r="S23" t="str">
-        <f>IF(NOT(K23=""),K23&amp;"|"&amp;A23,"")</f>
+        <f t="shared" si="4"/>
         <v>517-9691020000DA|5</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23">
+      <c r="A24" s="21">
         <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2761,7 +2757,7 @@
         <v>57</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L24" s="5">
         <v>0.56000000000000005</v>
@@ -2781,20 +2777,20 @@
         <v>89</v>
       </c>
       <c r="Q24" s="4" t="str">
-        <f>IF(NOT(J24=""),A24&amp;","&amp;J24,"")</f>
+        <f t="shared" si="0"/>
         <v>4,S1012EC-40-ND</v>
       </c>
       <c r="R24" t="str">
-        <f>A24&amp;"x "&amp;C24</f>
+        <f t="shared" si="10"/>
         <v>4x 40 POS 0.100 Pin Header</v>
       </c>
       <c r="S24" t="str">
-        <f>IF(NOT(K24=""),K24&amp;"|"&amp;A24,"")</f>
+        <f t="shared" si="4"/>
         <v>855-M20-9774046|4</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2811,20 +2807,20 @@
       <c r="O25" s="6"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="str">
-        <f>IF(NOT(J25=""),A25&amp;","&amp;J25,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="R25" t="str">
-        <f>A25&amp;"x "&amp;C25</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">x </v>
       </c>
       <c r="S25" t="str">
-        <f>IF(NOT(K25=""),K25&amp;"|"&amp;A25,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23">
+      <c r="A26" s="21">
         <f>LEN(B26)-LEN(SUBSTITUTE(B26,",",""))+1</f>
         <v>2</v>
       </c>
@@ -2832,27 +2828,27 @@
         <v>67</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="L26" s="5">
         <v>1.65</v>
@@ -2870,50 +2866,50 @@
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="str">
-        <f>IF(NOT(J26=""),A26&amp;","&amp;J26,"")</f>
+        <f t="shared" si="0"/>
         <v>2, TC4424AVOA-ND</v>
       </c>
       <c r="R26" t="str">
-        <f>A26&amp;"x "&amp;C26</f>
+        <f t="shared" si="10"/>
         <v>2x 3A</v>
       </c>
       <c r="S26" t="str">
-        <f>IF(NOT(K26=""),K26&amp;"|"&amp;A26,"")</f>
+        <f t="shared" si="4"/>
         <v>579-TC4424AVOA|2</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
+      <c r="A27" s="21">
         <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
         <v>3</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="L27" s="5">
         <v>1.65</v>
@@ -2931,48 +2927,48 @@
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="str">
-        <f>IF(NOT(J27=""),A27&amp;","&amp;J27,"")</f>
+        <f t="shared" si="0"/>
         <v>3,VNLD5090-E-ND</v>
       </c>
       <c r="R27" t="str">
-        <f>A27&amp;"x "&amp;C27</f>
+        <f t="shared" si="10"/>
         <v>3x 13A</v>
       </c>
       <c r="S27" t="str">
-        <f>IF(NOT(K27=""),K27&amp;"|"&amp;A27,"")</f>
+        <f t="shared" si="4"/>
         <v>511-VNLD5090-E|3</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
+      <c r="A28" s="21">
         <f>LEN(B28)-LEN(SUBSTITUTE(B28,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L28" s="5">
         <v>3.34</v>
@@ -2990,48 +2986,48 @@
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="str">
-        <f>IF(NOT(J28=""),A28&amp;","&amp;J28,"")</f>
+        <f t="shared" si="0"/>
         <v>1,F3162CT-ND</v>
       </c>
       <c r="R28" t="str">
-        <f>A28&amp;"x "&amp;C28</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">1x </v>
       </c>
       <c r="S28" t="str">
-        <f>IF(NOT(K28=""),K28&amp;"|"&amp;A28,"")</f>
+        <f t="shared" si="4"/>
         <v>576-SP720ABTG|1</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23">
+    <row r="29" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21">
         <f>LEN(B29)-LEN(SUBSTITUTE(B29,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>196</v>
+        <v>255</v>
       </c>
       <c r="L29" s="5">
         <v>5.2</v>
@@ -3049,20 +3045,20 @@
       </c>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="str">
-        <f>IF(NOT(J29=""),A29&amp;","&amp;J29,"")</f>
+        <f t="shared" si="0"/>
         <v>1,MC33814AE-ND</v>
       </c>
       <c r="R29" t="str">
-        <f>A29&amp;"x "&amp;C29</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">1x </v>
       </c>
       <c r="S29" t="str">
-        <f>IF(NOT(K29=""),K29&amp;"|"&amp;A29,"")</f>
-        <v>841-MC33814AE_x000D_|1</v>
+        <f t="shared" si="4"/>
+        <v>841-MC33814AE|1</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -3079,16 +3075,16 @@
       <c r="O30" s="6"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="str">
-        <f>IF(NOT(J30=""),A30&amp;","&amp;J30,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S30" t="str">
-        <f>IF(NOT(K30=""),K30&amp;"|"&amp;A30,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -3105,30 +3101,30 @@
       <c r="O31" s="6"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="str">
-        <f>IF(NOT(J31=""),A31&amp;","&amp;J31,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S31" t="str">
-        <f>IF(NOT(K31=""),K31&amp;"|"&amp;A31,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23">
-        <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
+      <c r="A32" s="21">
+        <f t="shared" ref="A32:A40" si="11">LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>206</v>
+        <v>198</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>200</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
@@ -3138,13 +3134,13 @@
         <v>71</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="L32" s="5">
         <v>0.39</v>
@@ -3153,40 +3149,40 @@
         <v>0.39</v>
       </c>
       <c r="N32" s="6">
-        <f>L32*A32</f>
+        <f t="shared" ref="N32:N40" si="12">L32*A32</f>
         <v>0.78</v>
       </c>
       <c r="O32" s="6">
-        <f>M32*A32</f>
+        <f t="shared" ref="O32:O40" si="13">M32*A32</f>
         <v>0.78</v>
       </c>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="str">
-        <f>IF(NOT(J32=""),A32&amp;","&amp;J32,"")</f>
+        <f t="shared" si="0"/>
         <v>2,YAG1854CT-ND</v>
       </c>
       <c r="R32" t="str">
-        <f>"Resistor - " &amp; A32&amp;"x "&amp;C32</f>
+        <f t="shared" ref="R32:R40" si="14">"Resistor - " &amp; A32&amp;"x "&amp;C32</f>
         <v>Resistor - 2x 2.49k</v>
       </c>
       <c r="S32" t="str">
-        <f>IF(NOT(K32=""),K32&amp;"|"&amp;A32,"")</f>
+        <f t="shared" si="4"/>
         <v>603-RT0805BRD072K49L|2</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23">
-        <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
+      <c r="A33" s="21">
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C33" s="3">
         <v>470</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -3197,13 +3193,13 @@
         <v>71</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="L33" s="5">
         <v>0.1</v>
@@ -3212,40 +3208,40 @@
         <v>0.1</v>
       </c>
       <c r="N33" s="6">
-        <f>L33*A33</f>
+        <f t="shared" si="12"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="O33" s="6">
-        <f>M33*A33</f>
+        <f t="shared" si="13"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="str">
-        <f>IF(NOT(J33=""),A33&amp;","&amp;J33,"")</f>
+        <f t="shared" si="0"/>
         <v>6,P470CCT-ND</v>
       </c>
       <c r="R33" t="str">
-        <f>"Resistor - " &amp; A33&amp;"x "&amp;C33</f>
+        <f t="shared" si="14"/>
         <v>Resistor - 6x 470</v>
       </c>
       <c r="S33" t="str">
-        <f>IF(NOT(K33=""),K33&amp;"|"&amp;A33,"")</f>
+        <f t="shared" si="4"/>
         <v>667-ERJ-6ENF4700V|6</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="23">
-        <f>LEN(B34)-LEN(SUBSTITUTE(B34,",",""))+1</f>
+      <c r="A34" s="21">
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="13"/>
@@ -3256,13 +3252,13 @@
         <v>71</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="L34" s="14">
         <v>0.1</v>
@@ -3271,40 +3267,40 @@
         <v>0.1</v>
       </c>
       <c r="N34" s="6">
-        <f>L34*A34</f>
+        <f t="shared" si="12"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="O34" s="6">
-        <f>M34*A34</f>
+        <f t="shared" si="13"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="P34" s="12"/>
       <c r="Q34" s="4" t="str">
-        <f>IF(NOT(J34=""),A34&amp;","&amp;J34,"")</f>
+        <f t="shared" si="0"/>
         <v>14,311-1.00KCRCT-ND</v>
       </c>
       <c r="R34" t="str">
-        <f>"Resistor - " &amp; A34&amp;"x "&amp;C34</f>
+        <f t="shared" si="14"/>
         <v>Resistor - 14x 1k</v>
       </c>
       <c r="S34" t="str">
-        <f>IF(NOT(K34=""),K34&amp;"|"&amp;A34,"")</f>
+        <f t="shared" si="4"/>
         <v>603-RC0805FR-071KL|14</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="23">
-        <f>LEN(B35)-LEN(SUBSTITUTE(B35,",",""))+1</f>
+      <c r="A35" s="21">
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -3315,13 +3311,13 @@
         <v>71</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="L35" s="5">
         <v>0.1</v>
@@ -3330,40 +3326,40 @@
         <v>0.1</v>
       </c>
       <c r="N35" s="6">
-        <f>L35*A35</f>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="O35" s="6">
-        <f>M35*A35</f>
+        <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="str">
-        <f>IF(NOT(J35=""),A35&amp;","&amp;J35,"")</f>
+        <f t="shared" si="0"/>
         <v>1,311-3.90KCRCT-ND</v>
       </c>
       <c r="R35" t="str">
-        <f>"Resistor - " &amp; A35&amp;"x "&amp;C35</f>
+        <f t="shared" si="14"/>
         <v>Resistor - 1x 3.9k</v>
       </c>
       <c r="S35" t="str">
-        <f>IF(NOT(K35=""),K35&amp;"|"&amp;A35,"")</f>
+        <f t="shared" si="4"/>
         <v>603-RC0805FR-073K9L|1</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23">
-        <f>LEN(B36)-LEN(SUBSTITUTE(B36,",",""))+1</f>
+      <c r="A36" s="21">
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -3374,13 +3370,13 @@
         <v>71</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="L36" s="5">
         <v>0.1</v>
@@ -3389,40 +3385,40 @@
         <v>0.1</v>
       </c>
       <c r="N36" s="6">
-        <f>L36*A36</f>
+        <f t="shared" si="12"/>
         <v>0.8</v>
       </c>
       <c r="O36" s="6">
-        <f>M36*A36</f>
+        <f t="shared" si="13"/>
         <v>0.8</v>
       </c>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="str">
-        <f>IF(NOT(J36=""),A36&amp;","&amp;J36,"")</f>
+        <f t="shared" si="0"/>
         <v>8,311-2.40KCRCT-ND</v>
       </c>
       <c r="R36" t="str">
-        <f>"Resistor - " &amp; A36&amp;"x "&amp;C36</f>
+        <f t="shared" si="14"/>
         <v>Resistor - 8x 2.4k</v>
       </c>
       <c r="S36" t="str">
-        <f>IF(NOT(K36=""),K36&amp;"|"&amp;A36,"")</f>
+        <f t="shared" si="4"/>
         <v>603-RC0805FR-072K4L|8</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="23">
-        <f>LEN(B37)-LEN(SUBSTITUTE(B37,",",""))+1</f>
+      <c r="A37" s="21">
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -3433,13 +3429,13 @@
         <v>71</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="L37" s="5">
         <v>0.1</v>
@@ -3448,40 +3444,40 @@
         <v>0.1</v>
       </c>
       <c r="N37" s="6">
-        <f>L37*A37</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="O37" s="6">
-        <f>M37*A37</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="str">
-        <f>IF(NOT(J37=""),A37&amp;","&amp;J37,"")</f>
+        <f t="shared" si="0"/>
         <v>10,311-100KCRCT-ND</v>
       </c>
       <c r="R37" t="str">
-        <f>"Resistor - " &amp; A37&amp;"x "&amp;C37</f>
+        <f t="shared" si="14"/>
         <v>Resistor - 10x 100k</v>
       </c>
       <c r="S37" t="str">
-        <f>IF(NOT(K37=""),K37&amp;"|"&amp;A37,"")</f>
+        <f t="shared" si="4"/>
         <v>603-RC0805FR-07100KL|10</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23">
-        <f>LEN(B38)-LEN(SUBSTITUTE(B38,",",""))+1</f>
+      <c r="A38" s="21">
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C38" s="3">
         <v>220</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -3492,13 +3488,13 @@
         <v>71</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="L38" s="5">
         <v>0.1</v>
@@ -3507,40 +3503,40 @@
         <v>0.1</v>
       </c>
       <c r="N38" s="6">
-        <f>L38*A38</f>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="O38" s="6">
-        <f>M38*A38</f>
+        <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="str">
-        <f>IF(NOT(J38=""),A38&amp;","&amp;J38,"")</f>
+        <f t="shared" si="0"/>
         <v>2,311-220CRCT-ND</v>
       </c>
       <c r="R38" t="str">
-        <f>"Resistor - " &amp; A38&amp;"x "&amp;C38</f>
+        <f t="shared" si="14"/>
         <v>Resistor - 2x 220</v>
       </c>
       <c r="S38" t="str">
-        <f>IF(NOT(K38=""),K38&amp;"|"&amp;A38,"")</f>
+        <f t="shared" si="4"/>
         <v>603-RC0805FR-07220RL|2</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="23">
-        <f>LEN(B39)-LEN(SUBSTITUTE(B39,",",""))+1</f>
+      <c r="A39" s="21">
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -3551,13 +3547,13 @@
         <v>71</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="L39" s="5">
         <v>0.1</v>
@@ -3566,40 +3562,40 @@
         <v>0.1</v>
       </c>
       <c r="N39" s="6">
-        <f>L39*A39</f>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="O39" s="6">
-        <f>M39*A39</f>
+        <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="str">
-        <f>IF(NOT(J39=""),A39&amp;","&amp;J39,"")</f>
+        <f t="shared" si="0"/>
         <v>1,311-10KARCT-ND</v>
       </c>
       <c r="R39" t="str">
-        <f>"Resistor - " &amp; A39&amp;"x "&amp;C39</f>
+        <f t="shared" si="14"/>
         <v>Resistor - 1x 10k</v>
       </c>
       <c r="S39" t="str">
-        <f>IF(NOT(K39=""),K39&amp;"|"&amp;A39,"")</f>
+        <f t="shared" si="4"/>
         <v>603-RC0805JR-0710KL|1</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23">
-        <f>LEN(B40)-LEN(SUBSTITUTE(B40,",",""))+1</f>
+      <c r="A40" s="21">
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C40" s="3">
         <v>10</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -3610,13 +3606,13 @@
         <v>71</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="L40" s="5">
         <v>0.1</v>
@@ -3625,29 +3621,29 @@
         <v>0.1</v>
       </c>
       <c r="N40" s="6">
-        <f>L40*A40</f>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="O40" s="6">
-        <f>M40*A40</f>
+        <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="str">
-        <f>IF(NOT(J40=""),A40&amp;","&amp;J40,"")</f>
+        <f t="shared" si="0"/>
         <v>2,311-10.0CRCT-ND</v>
       </c>
       <c r="R40" t="str">
-        <f>"Resistor - " &amp; A40&amp;"x "&amp;C40</f>
+        <f t="shared" si="14"/>
         <v>Resistor - 2x 10</v>
       </c>
       <c r="S40" t="str">
-        <f>IF(NOT(K40=""),K40&amp;"|"&amp;A40,"")</f>
+        <f t="shared" si="4"/>
         <v>603-RC0805FR-0710RL|2</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -3664,16 +3660,16 @@
       <c r="O41" s="6"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="str">
-        <f>IF(NOT(J41=""),A41&amp;","&amp;J41,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S41" t="str">
-        <f>IF(NOT(K41=""),K41&amp;"|"&amp;A41,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="4"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -3690,16 +3686,16 @@
       <c r="O42" s="6"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="str">
-        <f>IF(NOT(J42=""),A42&amp;","&amp;J42,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S42" t="str">
-        <f>IF(NOT(K42=""),K42&amp;"|"&amp;A42,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23">
+      <c r="A43" s="21">
         <v>1</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -3744,7 +3740,7 @@
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="str">
-        <f>IF(NOT(J43=""),A43&amp;","&amp;J43,"")</f>
+        <f t="shared" si="0"/>
         <v>1,MPX4250AP-ND</v>
       </c>
       <c r="R43" t="str">
@@ -3752,12 +3748,12 @@
         <v>1x 1-Bar MAP sensor</v>
       </c>
       <c r="S43" t="str">
-        <f>IF(NOT(K43=""),K43&amp;"|"&amp;A43,"")</f>
+        <f t="shared" si="4"/>
         <v>841-MPX4250AP|1</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="4"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -3774,16 +3770,16 @@
       <c r="O44" s="6"/>
       <c r="P44" s="10"/>
       <c r="Q44" s="4" t="str">
-        <f>IF(NOT(J44=""),A44&amp;","&amp;J44,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S44" t="str">
-        <f>IF(NOT(K44=""),K44&amp;"|"&amp;A44,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="23">
+    <row r="45" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="21">
         <v>1</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -3822,16 +3818,16 @@
       </c>
       <c r="P45" s="10"/>
       <c r="Q45" s="4" t="str">
-        <f>IF(NOT(J45=""),A45&amp;","&amp;J45,"")</f>
+        <f t="shared" si="0"/>
         <v>1,HM975-ND</v>
       </c>
       <c r="S45" t="str">
-        <f>IF(NOT(K45=""),K45&amp;"|"&amp;A45,"")</f>
+        <f t="shared" si="4"/>
         <v>546-1455N1202|1</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -3848,12 +3844,12 @@
       <c r="O46" s="6"/>
       <c r="P46" s="10"/>
       <c r="Q46" s="4" t="str">
-        <f>IF(NOT(J46=""),A46&amp;","&amp;J46,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="4" t="s">
         <v>37</v>
       </c>
@@ -3872,12 +3868,12 @@
       <c r="O47" s="6"/>
       <c r="P47" s="4"/>
       <c r="Q47" s="4" t="str">
-        <f>IF(NOT(J47=""),A47&amp;","&amp;J47,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="21">
+      <c r="A48" s="19">
         <v>1</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -3914,12 +3910,12 @@
       </c>
       <c r="P48" s="4"/>
       <c r="Q48" s="4" t="str">
-        <f>IF(NOT(J48=""),A48&amp;","&amp;J48,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="21">
+      <c r="A49" s="19">
         <v>1</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -3947,7 +3943,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="4"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -3955,10 +3951,10 @@
       <c r="F50" s="16"/>
       <c r="G50" s="4"/>
       <c r="H50" s="8"/>
-      <c r="I50" s="18" t="s">
+      <c r="I50" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="J50" s="19"/>
+      <c r="J50" s="24"/>
       <c r="K50" s="17"/>
       <c r="L50" s="1" t="s">
         <v>35</v>
@@ -3966,7 +3962,7 @@
       <c r="M50" s="1"/>
       <c r="N50" s="11">
         <f>SUM(N2:N49)</f>
-        <v>79.28</v>
+        <v>79</v>
       </c>
       <c r="O50" s="11">
         <f>SUM(O2:O49)</f>

</xml_diff>

<commit_message>
Cleanup of some design files for the MX5 board (PVT2)
</commit_message>
<xml_diff>
--- a/reference/hardware/Pro/MX5 PNP_BOM.xlsx
+++ b/reference/hardware/Pro/MX5 PNP_BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27211"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="270">
   <si>
     <t>Value</t>
   </si>
@@ -758,9 +758,6 @@
     <t>855-M20-9774046</t>
   </si>
   <si>
-    <t>C1,C3,C5,C7,C9,C22,C23</t>
-  </si>
-  <si>
     <t>C2,C4,C6,C8,C10</t>
   </si>
   <si>
@@ -795,6 +792,51 @@
   </si>
   <si>
     <t>841-MC33814AE</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>ZXTP07040DFF</t>
+  </si>
+  <si>
+    <t>TRANS PNP 40V 3A SOT23F-3</t>
+  </si>
+  <si>
+    <t>C1,C3,C5,C7,C9,C22,C23,C25</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>EEE-FK0J220R</t>
+  </si>
+  <si>
+    <t>22µF 6.3V Aluminum Capacitors Radial, Can - SMD 2000 Hrs @ 105°C</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>PCE3765CT-ND</t>
+  </si>
+  <si>
+    <t>667-EEE-FK0J220R</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>621-ZXTP07040DFFTA</t>
+  </si>
+  <si>
+    <t>ZXTP07040DFFCT-ND</t>
   </si>
 </sst>
 </file>
@@ -1450,10 +1492,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="95" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1548,7 +1590,7 @@
       <c r="O2" s="3"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4" t="str">
-        <f t="shared" ref="Q2:Q48" si="0">IF(NOT(J2=""),A2&amp;","&amp;J2,"")</f>
+        <f t="shared" ref="Q2:Q49" si="0">IF(NOT(J2=""),A2&amp;","&amp;J2,"")</f>
         <v/>
       </c>
       <c r="R2" t="str">
@@ -1559,16 +1601,16 @@
     <row r="3" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
@@ -1581,13 +1623,13 @@
         <v>71</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="L3" s="5">
         <v>0.1</v>
@@ -1596,25 +1638,25 @@
         <v>0.1</v>
       </c>
       <c r="N3" s="6">
-        <f t="shared" ref="N3:N11" si="1">L3*A3</f>
-        <v>0.70000000000000007</v>
+        <f t="shared" ref="N3:N12" si="1">L3*A3</f>
+        <v>0.8</v>
       </c>
       <c r="O3" s="6">
-        <f t="shared" ref="O3:O11" si="2">M3*A3</f>
-        <v>0.70000000000000007</v>
+        <f t="shared" ref="O3:O12" si="2">M3*A3</f>
+        <v>0.8</v>
       </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>7,311-1140-1-ND</v>
+        <v>8,311-1140-1-ND</v>
       </c>
       <c r="R3" t="str">
-        <f t="shared" ref="R3:R11" si="3">"Capacitor - " &amp;A3&amp;"x "&amp;C3</f>
-        <v>Capacitor - 7x 0.1uF / 100nF</v>
+        <f t="shared" ref="R3:R12" si="3">"Capacitor - " &amp;A3&amp;"x "&amp;C3</f>
+        <v>Capacitor - 8x 0.1uF / 100nF</v>
       </c>
       <c r="S3" t="str">
-        <f t="shared" ref="S3:S45" si="4">IF(NOT(K3=""),K3&amp;"|"&amp;A3,"")</f>
-        <v>603-CC805KRX7R9BB104|7</v>
+        <f t="shared" ref="S3:S46" si="4">IF(NOT(K3=""),K3&amp;"|"&amp;A3,"")</f>
+        <v>603-CC805KRX7R9BB104|8</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1623,7 +1665,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -1745,7 +1787,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -1806,7 +1848,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>113</v>
@@ -1867,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
@@ -2106,108 +2148,106 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="A12" s="21">
+        <f>LEN(B12)-LEN(SUBSTITUTE(B12,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>263</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="6"/>
+      <c r="G12" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0.36</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="2"/>
+        <v>0.36</v>
+      </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1,PCE3765CT-ND</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="3"/>
+        <v>Capacitor - 1x 22uF</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>667-EEE-FK0J220R|1</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
-        <f t="shared" ref="A13:A18" si="6">LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
-        <v>2</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="A13" s="19"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L13" s="5">
-        <v>0.34</v>
-      </c>
-      <c r="M13" s="5">
-        <v>0.43</v>
-      </c>
-      <c r="N13" s="6">
-        <f t="shared" ref="N13:N18" si="7">L13*A13</f>
-        <v>0.68</v>
-      </c>
-      <c r="O13" s="6">
-        <f t="shared" ref="O13:O18" si="8">M13*A13</f>
-        <v>0.86</v>
-      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="6"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2,1N5919BGOS-ND</v>
-      </c>
-      <c r="R13" t="str">
-        <f t="shared" ref="R13:R18" si="9">"Diode - " &amp;A13&amp;"x "&amp;C13</f>
-        <v>Diode - 2x 5.6V Zener</v>
+        <v/>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="4"/>
-        <v>863-1N5919BRLG|2</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="A14:A19" si="6">LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>141</v>
+        <v>14</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
@@ -2216,201 +2256,201 @@
       <c r="H14" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>137</v>
+      <c r="I14" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>142</v>
+        <v>90</v>
       </c>
       <c r="L14" s="5">
-        <v>0.14000000000000001</v>
+        <v>0.34</v>
       </c>
       <c r="M14" s="5">
-        <v>0.14000000000000001</v>
+        <v>0.43</v>
       </c>
       <c r="N14" s="6">
-        <f t="shared" si="7"/>
-        <v>0.28000000000000003</v>
+        <f t="shared" ref="N14:N19" si="7">L14*A14</f>
+        <v>0.68</v>
       </c>
       <c r="O14" s="6">
-        <f t="shared" si="8"/>
-        <v>0.28000000000000003</v>
+        <f t="shared" ref="O14:O19" si="8">M14*A14</f>
+        <v>0.86</v>
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2,MM3Z5V1ST1GOSCT-ND</v>
+        <v>2,1N5919BGOS-ND</v>
       </c>
       <c r="R14" t="str">
-        <f t="shared" si="9"/>
-        <v>Diode - 2x 5.1V Zener</v>
+        <f t="shared" ref="R14:R19" si="9">"Diode - " &amp;A14&amp;"x "&amp;C14</f>
+        <v>Diode - 2x 5.6V Zener</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="4"/>
-        <v>863-MM3Z5V1ST1G|2</v>
+        <v>863-1N5919BRLG|2</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>248</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="D15" s="3" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>141</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>147</v>
+        <v>15</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="L15" s="5">
         <v>0.14000000000000001</v>
       </c>
       <c r="M15" s="5">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="N15" s="6">
         <f t="shared" si="7"/>
-        <v>0.56000000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="O15" s="6">
         <f t="shared" si="8"/>
-        <v>0.52</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>4,1N4448WXTPMSCT-ND</v>
+        <v>2,MM3Z5V1ST1GOSCT-ND</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">Diode - 4x </v>
+        <v>Diode - 2x 5.1V Zener</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="4"/>
-        <v>833-1N4448WX-TP|4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+        <v>863-MM3Z5V1ST1G|2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>66</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>19</v>
+        <v>148</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>14</v>
+        <v>141</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>18</v>
+        <v>144</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>84</v>
+        <v>146</v>
       </c>
       <c r="L16" s="5">
-        <v>0.39</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M16" s="5">
-        <v>0.39</v>
+        <v>0.13</v>
       </c>
       <c r="N16" s="6">
         <f t="shared" si="7"/>
-        <v>0.39</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="O16" s="6">
         <f t="shared" si="8"/>
-        <v>0.39</v>
+        <v>0.52</v>
       </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1,1N5818-TPCT-ND</v>
+        <v>4,1N4448WXTPMSCT-ND</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" si="9"/>
-        <v>Diode - 1x 1N5818-TP Schottky</v>
+        <v xml:space="preserve">Diode - 4x </v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="4"/>
-        <v>833-1N5818-TP|1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>833-1N4448WX-TP|4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>156</v>
+        <v>66</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>155</v>
+        <v>19</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>141</v>
+        <v>14</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>72</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>151</v>
+        <v>18</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>152</v>
+        <v>21</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="L17" s="5">
         <v>0.39</v>
       </c>
       <c r="M17" s="5">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="N17" s="6">
         <f t="shared" si="7"/>
@@ -2418,584 +2458,586 @@
       </c>
       <c r="O17" s="6">
         <f t="shared" si="8"/>
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1,B0540WSDICT-ND</v>
+        <v>1,1N5818-TPCT-ND</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" si="9"/>
-        <v>Diode - 1x Schottky</v>
+        <v>Diode - 1x 1N5818-TP Schottky</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="4"/>
-        <v>621-B0540WS-7|1</v>
+        <v>833-1N5818-TP|1</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>43</v>
+        <v>150</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E18" s="3">
-        <v>805</v>
+        <v>155</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>72</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L18" s="5">
-        <v>0.26</v>
+        <v>0.39</v>
       </c>
       <c r="M18" s="5">
-        <v>0.24</v>
+        <v>0.41</v>
       </c>
       <c r="N18" s="6">
         <f t="shared" si="7"/>
-        <v>2.08</v>
+        <v>0.39</v>
       </c>
       <c r="O18" s="6">
         <f t="shared" si="8"/>
-        <v>1.92</v>
+        <v>0.41</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>8,475-1415-1-ND</v>
+        <v>1,B0540WSDICT-ND</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" si="9"/>
-        <v>Diode - 8x LED-Red</v>
+        <v>Diode - 1x Schottky</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 720-LHR974-LP-1|8</v>
+        <v>621-B0540WS-7|1</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="21">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E19" s="3">
+        <v>805</v>
+      </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="6"/>
+      <c r="G19" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L19" s="5">
+        <v>0.26</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0.24</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" si="7"/>
+        <v>2.08</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" si="8"/>
+        <v>1.92</v>
+      </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>8,475-1415-1-ND</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" ref="R19:R29" si="10">A19&amp;"x "&amp;C19</f>
-        <v xml:space="preserve">x </v>
+        <f t="shared" si="9"/>
+        <v>Diode - 8x LED-Red</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v xml:space="preserve"> 720-LHR974-LP-1|8</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A20" s="19"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L20" s="5">
-        <v>0.72</v>
-      </c>
-      <c r="M20" s="5">
-        <v>0.72</v>
-      </c>
-      <c r="N20" s="6">
-        <f>L20*A20</f>
-        <v>0.72</v>
-      </c>
-      <c r="O20" s="6">
-        <f>M20*A20</f>
-        <v>0.72</v>
-      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="6"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="R20" t="str">
+        <f t="shared" ref="R20:R30" si="10">A20&amp;"x "&amp;C20</f>
+        <v xml:space="preserve">x </v>
+      </c>
+      <c r="S20" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L21" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="M21" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="N21" s="6">
+        <f>L21*A21</f>
+        <v>0.72</v>
+      </c>
+      <c r="O21" s="6">
+        <f>M21*A21</f>
+        <v>0.72</v>
+      </c>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>1,P7307-ND</v>
       </c>
-      <c r="R20" t="str">
+      <c r="R21" t="str">
         <f t="shared" si="10"/>
         <v>1x Surge Protection</v>
       </c>
-      <c r="S20" t="str">
+      <c r="S21" t="str">
         <f t="shared" si="4"/>
         <v>667-ERZ-V14D220|1</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4" t="str">
+    <row r="22" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R21" t="str">
+      <c r="R22" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">x </v>
       </c>
-      <c r="S21" t="str">
+      <c r="S22" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
+    <row r="23" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
         <v>1</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="L22" s="5">
+      <c r="L23" s="5">
         <v>9.06</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M23" s="5">
         <v>7.82</v>
       </c>
-      <c r="N22" s="6">
-        <f>L22*A22</f>
+      <c r="N23" s="6">
+        <f>L23*A23</f>
         <v>9.06</v>
       </c>
-      <c r="O22" s="6">
-        <f>M22*A22</f>
+      <c r="O23" s="6">
+        <f>M23*A23</f>
         <v>7.82</v>
       </c>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4" t="str">
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1,174917-7-ND</v>
       </c>
-      <c r="R22" t="str">
+      <c r="R23" t="str">
         <f t="shared" si="10"/>
         <v>1x Denso-48</v>
       </c>
-      <c r="S22" t="str">
+      <c r="S23" t="str">
         <f t="shared" si="4"/>
         <v>571-174917-7|1</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+    <row r="24" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21">
         <v>5</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L24" s="5">
         <v>0.1</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M24" s="5">
         <v>0.1</v>
       </c>
-      <c r="N23" s="6">
-        <f>L23*A23</f>
+      <c r="N24" s="6">
+        <f>L24*A24</f>
         <v>0.5</v>
       </c>
-      <c r="O23" s="6">
-        <f>M23*A23</f>
+      <c r="O24" s="6">
+        <f>M24*A24</f>
         <v>0.5</v>
       </c>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4" t="str">
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>5,3M9580-ND</v>
       </c>
-      <c r="R23" t="str">
+      <c r="R24" t="str">
         <f t="shared" si="10"/>
         <v>5x Jumper</v>
       </c>
-      <c r="S23" t="str">
+      <c r="S24" t="str">
         <f t="shared" si="4"/>
         <v>517-9691020000DA|5</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21">
+    <row r="25" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
         <v>4</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3" t="s">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L25" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M25" s="5">
         <v>1.21</v>
       </c>
-      <c r="N24" s="6">
-        <f>L24*A24</f>
+      <c r="N25" s="6">
+        <f>L25*A25</f>
         <v>2.2400000000000002</v>
       </c>
-      <c r="O24" s="6">
-        <f>M24*A24</f>
+      <c r="O25" s="6">
+        <f>M25*A25</f>
         <v>4.84</v>
       </c>
-      <c r="P24" s="4" t="s">
+      <c r="P25" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="Q24" s="4" t="str">
+      <c r="Q25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>4,S1012EC-40-ND</v>
       </c>
-      <c r="R24" t="str">
+      <c r="R25" t="str">
         <f t="shared" si="10"/>
         <v>4x 40 POS 0.100 Pin Header</v>
       </c>
-      <c r="S24" t="str">
+      <c r="S25" t="str">
         <f t="shared" si="4"/>
         <v>855-M20-9774046|4</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4" t="str">
+    <row r="26" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R25" t="str">
+      <c r="R26" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">x </v>
       </c>
-      <c r="S25" t="str">
+      <c r="S26" t="str">
         <f t="shared" si="4"/>
         <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21">
-        <f>LEN(B26)-LEN(SUBSTITUTE(B26,",",""))+1</f>
-        <v>2</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="L26" s="5">
-        <v>1.65</v>
-      </c>
-      <c r="M26" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="N26" s="6">
-        <f>L26*A26</f>
-        <v>3.3</v>
-      </c>
-      <c r="O26" s="6">
-        <f>M26*A26</f>
-        <v>3.6</v>
-      </c>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>2, TC4424AVOA-ND</v>
-      </c>
-      <c r="R26" t="str">
-        <f t="shared" si="10"/>
-        <v>2x 3A</v>
-      </c>
-      <c r="S26" t="str">
-        <f t="shared" si="4"/>
-        <v>579-TC4424AVOA|2</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>181</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="L27" s="5">
         <v>1.65</v>
       </c>
       <c r="M27" s="5">
-        <v>1.65</v>
+        <v>1.8</v>
       </c>
       <c r="N27" s="6">
         <f>L27*A27</f>
-        <v>4.9499999999999993</v>
+        <v>3.3</v>
       </c>
       <c r="O27" s="6">
         <f>M27*A27</f>
-        <v>4.9499999999999993</v>
+        <v>3.6</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>3,VNLD5090-E-ND</v>
+        <v>2, TC4424AVOA-ND</v>
       </c>
       <c r="R27" t="str">
         <f t="shared" si="10"/>
-        <v>3x 13A</v>
+        <v>2x 3A</v>
       </c>
       <c r="S27" t="str">
         <f t="shared" si="4"/>
-        <v>511-VNLD5090-E|3</v>
+        <v>579-TC4424AVOA|2</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <f>LEN(B28)-LEN(SUBSTITUTE(B28,",",""))+1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C28" s="3"/>
+        <v>174</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="D28" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="L28" s="5">
-        <v>3.34</v>
+        <v>1.65</v>
       </c>
       <c r="M28" s="5">
-        <v>3.34</v>
+        <v>1.65</v>
       </c>
       <c r="N28" s="6">
         <f>L28*A28</f>
-        <v>3.34</v>
+        <v>4.9499999999999993</v>
       </c>
       <c r="O28" s="6">
         <f>M28*A28</f>
-        <v>3.34</v>
+        <v>4.9499999999999993</v>
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1,F3162CT-ND</v>
+        <v>3,VNLD5090-E-ND</v>
       </c>
       <c r="R28" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">1x </v>
+        <v>3x 13A</v>
       </c>
       <c r="S28" t="str">
         <f t="shared" si="4"/>
-        <v>576-SP720ABTG|1</v>
+        <v>511-VNLD5090-E|3</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3004,49 +3046,49 @@
         <v>1</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>255</v>
+        <v>185</v>
       </c>
       <c r="L29" s="5">
-        <v>5.2</v>
+        <v>3.34</v>
       </c>
       <c r="M29" s="5">
-        <v>5.2</v>
+        <v>3.34</v>
       </c>
       <c r="N29" s="6">
         <f>L29*A29</f>
-        <v>5.2</v>
+        <v>3.34</v>
       </c>
       <c r="O29" s="6">
         <f>M29*A29</f>
-        <v>5.2</v>
+        <v>3.34</v>
       </c>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1,MC33814AE-ND</v>
+        <v>1,F3162CT-ND</v>
       </c>
       <c r="R29" t="str">
         <f t="shared" si="10"/>
@@ -3054,272 +3096,301 @@
       </c>
       <c r="S29" t="str">
         <f t="shared" si="4"/>
-        <v>841-MC33814AE|1</v>
+        <v>576-SP720ABTG|1</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="21">
+        <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="6"/>
+      <c r="G30" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="L30" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="M30" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="N30" s="6">
+        <f>L30*A30</f>
+        <v>5.2</v>
+      </c>
+      <c r="O30" s="6">
+        <f>M30*A30</f>
+        <v>5.2</v>
+      </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1,MC33814AE-ND</v>
+      </c>
+      <c r="R30" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">1x </v>
       </c>
       <c r="S30" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>841-MC33814AE|1</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="21">
+        <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>255</v>
+      </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>256</v>
+      </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="6"/>
+      <c r="G31" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L31" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="M31" s="5">
+        <v>0.62</v>
+      </c>
+      <c r="N31" s="3">
+        <f>L31*A31</f>
+        <v>0.65</v>
+      </c>
+      <c r="O31" s="6">
+        <f>M31*A31</f>
+        <v>0.62</v>
+      </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1,ZXTP07040DFFCT-ND</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>621-ZXTP07040DFFTA|1</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21">
-        <f t="shared" ref="A32:A40" si="11">LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
-        <v>2</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>200</v>
-      </c>
+      <c r="A32" s="19"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="L32" s="5">
-        <v>0.39</v>
-      </c>
-      <c r="M32" s="5">
-        <v>0.39</v>
-      </c>
-      <c r="N32" s="6">
-        <f t="shared" ref="N32:N40" si="12">L32*A32</f>
-        <v>0.78</v>
-      </c>
-      <c r="O32" s="6">
-        <f t="shared" ref="O32:O40" si="13">M32*A32</f>
-        <v>0.78</v>
-      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="6"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2,YAG1854CT-ND</v>
-      </c>
-      <c r="R32" t="str">
-        <f t="shared" ref="R32:R40" si="14">"Resistor - " &amp; A32&amp;"x "&amp;C32</f>
-        <v>Resistor - 2x 2.49k</v>
+        <v/>
       </c>
       <c r="S32" t="str">
         <f t="shared" si="4"/>
-        <v>603-RT0805BRD072K49L|2</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
-        <f t="shared" si="11"/>
-        <v>6</v>
+        <f t="shared" ref="A33:A41" si="11">LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
+        <v>2</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="C33" s="3">
-        <v>470</v>
+        <v>41</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E33" s="3"/>
+        <v>198</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>200</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L33" s="5">
-        <v>0.1</v>
+        <v>0.39</v>
       </c>
       <c r="M33" s="5">
-        <v>0.1</v>
+        <v>0.39</v>
       </c>
       <c r="N33" s="6">
-        <f t="shared" si="12"/>
-        <v>0.60000000000000009</v>
+        <f t="shared" ref="N33:N41" si="12">L33*A33</f>
+        <v>0.78</v>
       </c>
       <c r="O33" s="6">
-        <f t="shared" si="13"/>
-        <v>0.60000000000000009</v>
+        <f t="shared" ref="O33:O41" si="13">M33*A33</f>
+        <v>0.78</v>
       </c>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>6,P470CCT-ND</v>
+        <v>2,YAG1854CT-ND</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="14"/>
-        <v>Resistor - 6x 470</v>
+        <f t="shared" ref="R33:R41" si="14">"Resistor - " &amp; A33&amp;"x "&amp;C33</f>
+        <v>Resistor - 2x 2.49k</v>
       </c>
       <c r="S33" t="str">
         <f t="shared" si="4"/>
-        <v>667-ERJ-6ENF4700V|6</v>
+        <v>603-RT0805BRD072K49L|2</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>210</v>
+        <v>6</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C34" s="3">
+        <v>470</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H34" s="13" t="s">
+      <c r="F34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="L34" s="14">
+        <v>204</v>
+      </c>
+      <c r="L34" s="5">
         <v>0.1</v>
       </c>
-      <c r="M34" s="14">
+      <c r="M34" s="5">
         <v>0.1</v>
       </c>
       <c r="N34" s="6">
         <f t="shared" si="12"/>
-        <v>1.4000000000000001</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="O34" s="6">
         <f t="shared" si="13"/>
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="P34" s="12"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="P34" s="4"/>
       <c r="Q34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>14,311-1.00KCRCT-ND</v>
+        <v>6,P470CCT-ND</v>
       </c>
       <c r="R34" t="str">
         <f t="shared" si="14"/>
-        <v>Resistor - 14x 1k</v>
+        <v>Resistor - 6x 470</v>
       </c>
       <c r="S34" t="str">
         <f t="shared" si="4"/>
-        <v>603-RC0805FR-071KL|14</v>
+        <v>667-ERJ-6ENF4700V|6</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>214</v>
+        <v>14</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3" t="s">
+      <c r="F35" s="13"/>
+      <c r="G35" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I35" s="7" t="s">
-        <v>211</v>
+      <c r="I35" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="L35" s="5">
+        <v>209</v>
+      </c>
+      <c r="L35" s="14">
         <v>0.1</v>
       </c>
       <c r="M35" s="14">
@@ -3327,39 +3398,39 @@
       </c>
       <c r="N35" s="6">
         <f t="shared" si="12"/>
-        <v>0.1</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="O35" s="6">
         <f t="shared" si="13"/>
-        <v>0.1</v>
-      </c>
-      <c r="P35" s="4"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="P35" s="12"/>
       <c r="Q35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1,311-3.90KCRCT-ND</v>
+        <v>14,311-1.00KCRCT-ND</v>
       </c>
       <c r="R35" t="str">
         <f t="shared" si="14"/>
-        <v>Resistor - 1x 3.9k</v>
+        <v>Resistor - 14x 1k</v>
       </c>
       <c r="S35" t="str">
         <f t="shared" si="4"/>
-        <v>603-RC0805FR-073K9L|1</v>
+        <v>603-RC0805FR-071KL|14</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>216</v>
+        <v>42</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -3369,56 +3440,56 @@
       <c r="H36" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>219</v>
+      <c r="I36" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L36" s="5">
         <v>0.1</v>
       </c>
-      <c r="M36" s="5">
+      <c r="M36" s="14">
         <v>0.1</v>
       </c>
       <c r="N36" s="6">
         <f t="shared" si="12"/>
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="O36" s="6">
         <f t="shared" si="13"/>
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>8,311-2.40KCRCT-ND</v>
+        <v>1,311-3.90KCRCT-ND</v>
       </c>
       <c r="R36" t="str">
         <f t="shared" si="14"/>
-        <v>Resistor - 8x 2.4k</v>
+        <v>Resistor - 1x 3.9k</v>
       </c>
       <c r="S36" t="str">
         <f t="shared" si="4"/>
-        <v>603-RC0805FR-072K4L|8</v>
+        <v>603-RC0805FR-073K9L|1</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>33</v>
+        <v>221</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -3429,13 +3500,13 @@
         <v>71</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="L37" s="5">
         <v>0.1</v>
@@ -3445,39 +3516,39 @@
       </c>
       <c r="N37" s="6">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="O37" s="6">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>10,311-100KCRCT-ND</v>
+        <v>8,311-2.40KCRCT-ND</v>
       </c>
       <c r="R37" t="str">
         <f t="shared" si="14"/>
-        <v>Resistor - 10x 100k</v>
+        <v>Resistor - 8x 2.4k</v>
       </c>
       <c r="S37" t="str">
         <f t="shared" si="4"/>
-        <v>603-RC0805FR-07100KL|10</v>
+        <v>603-RC0805FR-072K4L|8</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C38" s="3">
-        <v>220</v>
+        <v>222</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -3488,13 +3559,13 @@
         <v>71</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="L38" s="5">
         <v>0.1</v>
@@ -3504,39 +3575,39 @@
       </c>
       <c r="N38" s="6">
         <f t="shared" si="12"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="O38" s="6">
         <f t="shared" si="13"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2,311-220CRCT-ND</v>
+        <v>10,311-100KCRCT-ND</v>
       </c>
       <c r="R38" t="str">
         <f t="shared" si="14"/>
-        <v>Resistor - 2x 220</v>
+        <v>Resistor - 10x 100k</v>
       </c>
       <c r="S38" t="str">
         <f t="shared" si="4"/>
-        <v>603-RC0805FR-07220RL|2</v>
+        <v>603-RC0805FR-07100KL|10</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>30</v>
+        <v>227</v>
+      </c>
+      <c r="C39" s="3">
+        <v>220</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -3547,13 +3618,13 @@
         <v>71</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="L39" s="5">
         <v>0.1</v>
@@ -3563,39 +3634,39 @@
       </c>
       <c r="N39" s="6">
         <f t="shared" si="12"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="O39" s="6">
         <f t="shared" si="13"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1,311-10KARCT-ND</v>
+        <v>2,311-220CRCT-ND</v>
       </c>
       <c r="R39" t="str">
         <f t="shared" si="14"/>
-        <v>Resistor - 1x 10k</v>
+        <v>Resistor - 2x 220</v>
       </c>
       <c r="S39" t="str">
         <f t="shared" si="4"/>
-        <v>603-RC0805JR-0710KL|1</v>
+        <v>603-RC0805FR-07220RL|2</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C40" s="3">
-        <v>10</v>
+        <v>232</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -3606,13 +3677,13 @@
         <v>71</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="L40" s="5">
         <v>0.1</v>
@@ -3622,50 +3693,83 @@
       </c>
       <c r="N40" s="6">
         <f t="shared" si="12"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O40" s="6">
         <f t="shared" si="13"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2,311-10.0CRCT-ND</v>
+        <v>1,311-10KARCT-ND</v>
       </c>
       <c r="R40" t="str">
         <f t="shared" si="14"/>
-        <v>Resistor - 2x 10</v>
+        <v>Resistor - 1x 10k</v>
       </c>
       <c r="S40" t="str">
         <f t="shared" si="4"/>
-        <v>603-RC0805FR-0710RL|2</v>
+        <v>603-RC0805JR-0710KL|1</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="A41" s="21">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" s="3">
+        <v>10</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>237</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="6"/>
+      <c r="G41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="L41" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M41" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="N41" s="6">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="O41" s="6">
+        <f t="shared" si="13"/>
+        <v>0.2</v>
+      </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2,311-10.0CRCT-ND</v>
+      </c>
+      <c r="R41" t="str">
+        <f t="shared" si="14"/>
+        <v>Resistor - 2x 10</v>
       </c>
       <c r="S41" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>603-RC0805FR-0710RL|2</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3695,293 +3799,319 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21">
-        <v>1</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="A43" s="19"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L43" s="6">
-        <v>15.41</v>
-      </c>
-      <c r="M43" s="6">
-        <v>15.41</v>
-      </c>
-      <c r="N43" s="6">
-        <f>L43*A43</f>
-        <v>15.41</v>
-      </c>
-      <c r="O43" s="6">
-        <f>M43*A43</f>
-        <v>15.41</v>
-      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="6"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S43" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="21">
+        <v>1</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L44" s="6">
+        <v>15.41</v>
+      </c>
+      <c r="M44" s="6">
+        <v>15.41</v>
+      </c>
+      <c r="N44" s="6">
+        <f>L44*A44</f>
+        <v>15.41</v>
+      </c>
+      <c r="O44" s="6">
+        <f>M44*A44</f>
+        <v>15.41</v>
+      </c>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>1,MPX4250AP-ND</v>
       </c>
-      <c r="R43" t="str">
-        <f>A43&amp;"x "&amp;C43</f>
+      <c r="R44" t="str">
+        <f>A44&amp;"x "&amp;C44</f>
         <v>1x 1-Bar MAP sensor</v>
       </c>
-      <c r="S43" t="str">
+      <c r="S44" t="str">
         <f t="shared" si="4"/>
         <v>841-MPX4250AP|1</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S44" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
     <row r="45" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="21">
-        <v>1</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="A45" s="19"/>
+      <c r="B45" s="4"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J45" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="K45" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="L45" s="6">
-        <v>15.33</v>
-      </c>
-      <c r="M45" s="6">
-        <v>15.33</v>
-      </c>
-      <c r="N45" s="6">
-        <f>L45*A45</f>
-        <v>15.33</v>
-      </c>
-      <c r="O45" s="6">
-        <f>M45*A45</f>
-        <v>15.33</v>
-      </c>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="6"/>
       <c r="P45" s="10"/>
       <c r="Q45" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1,HM975-ND</v>
+        <v/>
       </c>
       <c r="S45" t="str">
         <f t="shared" si="4"/>
-        <v>546-1455N1202|1</v>
+        <v/>
       </c>
     </row>
     <row r="46" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="21">
+        <v>1</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="6"/>
+      <c r="G46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="K46" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="L46" s="6">
+        <v>15.33</v>
+      </c>
+      <c r="M46" s="6">
+        <v>15.33</v>
+      </c>
+      <c r="N46" s="6">
+        <f>L46*A46</f>
+        <v>15.33</v>
+      </c>
+      <c r="O46" s="6">
+        <f>M46*A46</f>
+        <v>15.33</v>
+      </c>
       <c r="P46" s="10"/>
       <c r="Q46" s="4" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1,HM975-ND</v>
+      </c>
+      <c r="S46" t="str">
+        <f t="shared" si="4"/>
+        <v>546-1455N1202|1</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
-      <c r="B47" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="B47" s="4"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="16"/>
+      <c r="F47" s="3"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="9"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="3"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="10"/>
       <c r="O47" s="6"/>
-      <c r="P47" s="4"/>
+      <c r="P47" s="10"/>
       <c r="Q47" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
-        <v>1</v>
-      </c>
+      <c r="A48" s="19"/>
       <c r="B48" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="F48" s="16"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="4"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
-      <c r="L48" s="6">
-        <v>4</v>
-      </c>
-      <c r="M48" s="6">
-        <v>4</v>
-      </c>
-      <c r="N48" s="6">
-        <f>L48*A48</f>
-        <v>4</v>
-      </c>
-      <c r="O48" s="6">
-        <f>M48*A48</f>
-        <v>4</v>
-      </c>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="6"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
         <v>1</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="I49" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J49" s="3"/>
       <c r="K49" s="3"/>
-      <c r="L49" s="3">
-        <v>61.65</v>
-      </c>
-      <c r="M49" s="3"/>
-      <c r="N49" s="6"/>
-      <c r="O49" s="6"/>
-      <c r="P49" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
-      <c r="B50" s="4"/>
+      <c r="L49" s="6">
+        <v>4</v>
+      </c>
+      <c r="M49" s="6">
+        <v>4</v>
+      </c>
+      <c r="N49" s="6">
+        <f>L49*A49</f>
+        <v>4</v>
+      </c>
+      <c r="O49" s="6">
+        <f>M49*A49</f>
+        <v>4</v>
+      </c>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="19">
+        <v>1</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="23" t="s">
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3">
+        <v>61.65</v>
+      </c>
+      <c r="M50" s="3"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="J50" s="24"/>
-      <c r="K50" s="17"/>
-      <c r="L50" s="1" t="s">
+      <c r="J51" s="24"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M50" s="1"/>
-      <c r="N50" s="11">
-        <f>SUM(N2:N49)</f>
-        <v>79</v>
-      </c>
-      <c r="O50" s="11">
-        <f>SUM(O2:O49)</f>
-        <v>80.42</v>
-      </c>
-      <c r="P50" s="10" t="s">
+      <c r="M51" s="1"/>
+      <c r="N51" s="11">
+        <f>SUM(N2:N50)</f>
+        <v>80.150000000000006</v>
+      </c>
+      <c r="O51" s="11">
+        <f>SUM(O2:O50)</f>
+        <v>81.500000000000014</v>
+      </c>
+      <c r="P51" s="10" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I51:J51"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J20" r:id="rId1"/>
-    <hyperlink ref="J43" r:id="rId2"/>
-    <hyperlink ref="J17" r:id="rId3" display="1N5818-TPCT-ND"/>
-    <hyperlink ref="J16" r:id="rId4"/>
+    <hyperlink ref="J21" r:id="rId1"/>
+    <hyperlink ref="J44" r:id="rId2"/>
+    <hyperlink ref="J18" r:id="rId3" display="1N5818-TPCT-ND"/>
+    <hyperlink ref="J17" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="35" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>